<commit_message>
updated several xl files, modified to PeRM data structure
</commit_message>
<xml_diff>
--- a/dataManagement/LiveData/reports_xlsx/On Hand and No Sales - IS version.xlsx
+++ b/dataManagement/LiveData/reports_xlsx/On Hand and No Sales - IS version.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\us160212\Documents\GitHub\PeRM\dataManagement\LiveData\reports_xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EADCECA8-31D8-442B-B7D6-FA5FDE1AC1B6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C1CB13F-ED7A-4EB5-9B4B-03E3FDBD4AEE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5220" yWindow="1058" windowWidth="16875" windowHeight="10522" xr2:uid="{639EC47F-865C-4631-846A-0A0068AD2729}"/>
+    <workbookView xWindow="442" yWindow="2678" windowWidth="22058" windowHeight="10522" activeTab="1" xr2:uid="{639EC47F-865C-4631-846A-0A0068AD2729}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="FILEPATH" sheetId="3" state="hidden" r:id="rId2"/>
+    <sheet name="verification" sheetId="4" r:id="rId2"/>
+    <sheet name="FILEPATH" sheetId="3" state="hidden" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Sheet2!$A$1:$H$1326</definedName>
@@ -100,7 +101,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3984" uniqueCount="1421">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3995" uniqueCount="1432">
   <si>
     <t>SKU</t>
   </si>
@@ -4363,6 +4364,39 @@
   </si>
   <si>
     <t>2X4-8FT #2 PT</t>
+  </si>
+  <si>
+    <t>indicators</t>
+  </si>
+  <si>
+    <t>all records have positive on-hand</t>
+  </si>
+  <si>
+    <t>aka - any blank or zero value for OH, will verify false</t>
+  </si>
+  <si>
+    <t>latest oh data is within trailing 7 days from today()</t>
+  </si>
+  <si>
+    <t>max oh date</t>
+  </si>
+  <si>
+    <t>today</t>
+  </si>
+  <si>
+    <t>diff</t>
+  </si>
+  <si>
+    <t>is within 7 days</t>
+  </si>
+  <si>
+    <t>record count</t>
+  </si>
+  <si>
+    <t>counta(oh date)</t>
+  </si>
+  <si>
+    <t>Column1</t>
   </si>
 </sst>
 </file>
@@ -4384,12 +4418,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -4404,15 +4444,73 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="12">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
     </dxf>
@@ -4441,6 +4539,228 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>4763</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E3252D7-558D-4F39-863E-023552F8D4AE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8377238" y="723900"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>223837</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>80963</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="6072303" cy="1297919"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F2F731DE-ED86-42B9-9DE6-25B95459CB0F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6005512" y="804863"/>
+          <a:ext cx="6072303" cy="1297919"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:lnRef>
+        <a:fillRef idx="2">
+          <a:schemeClr val="accent6"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent6"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" i="0" u="sng" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>indicators</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" b="1" u="sng"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- all records have positive on-hand</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- - aka - any blank or zero value for OH, will verify false</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- latest oh data is within trailing 7 days from today()</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>why</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng" baseline="0"/>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" u="sng"/>
+            <a:t>7 days?</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>  - if I refresh a report on a Sunday, I expect to see data from last week Sunday</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>this is because </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>I don't expect the latest POS data will be availalbe (</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100"/>
+            <a:t>for the whole week previous week)</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="ExternalData_1" connectionId="17" xr16:uid="{44FB6BCF-66A4-4883-B36E-0A957BB2595F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0">
   <queryTableRefresh nextId="23">
@@ -4462,16 +4782,55 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{70CC3F5D-E1F3-4209-A537-61F666C3A333}" name="OUTPUT" displayName="OUTPUT" ref="A1:H1326" tableType="queryTable" totalsRowShown="0">
   <autoFilter ref="A1:H1326" xr:uid="{514AC4C8-0F61-45BC-BB72-A13E74F373DF}"/>
   <tableColumns count="8">
-    <tableColumn id="1" xr3:uid="{B27052A8-1BC3-4EE1-BF64-835387D0AB45}" uniqueName="1" name="SKU" queryTableFieldId="8" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{6F676D2A-E8A1-4898-BD57-E6CB99E21B89}" uniqueName="2" name="STORE" queryTableFieldId="9" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{B27052A8-1BC3-4EE1-BF64-835387D0AB45}" uniqueName="1" name="SKU" queryTableFieldId="8" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{6F676D2A-E8A1-4898-BD57-E6CB99E21B89}" uniqueName="2" name="STORE" queryTableFieldId="9" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{C641C0D2-59BB-456E-8D3E-65FA5BFBAA4A}" uniqueName="4" name="OH" queryTableFieldId="10"/>
     <tableColumn id="7" xr3:uid="{CF110A6C-F8DE-41E9-B4FA-E9CE831FB710}" uniqueName="7" name="MKT_UNITS_T52WK" queryTableFieldId="17"/>
-    <tableColumn id="3" xr3:uid="{913DDE96-71A8-4139-8474-499E49F3791C}" uniqueName="3" name="OH_DATE" queryTableFieldId="3" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{913DDE96-71A8-4139-8474-499E49F3791C}" uniqueName="3" name="OH_DATE" queryTableFieldId="3" dataDxfId="9"/>
     <tableColumn id="8" xr3:uid="{03B87B1E-AEC2-42F2-A7AC-D941CD09C9FE}" uniqueName="8" name="MKT_SALES_T52WK" queryTableFieldId="18"/>
-    <tableColumn id="5" xr3:uid="{86ECD117-3EB9-46A5-A793-C1C615A6BF2A}" uniqueName="5" name="SKU_DESCRIPTION" queryTableFieldId="21" dataDxfId="1"/>
-    <tableColumn id="9" xr3:uid="{AE09184F-0511-4178-958B-3187FE75758F}" uniqueName="9" name="DATE_SUBMISSION" queryTableFieldId="20" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{86ECD117-3EB9-46A5-A793-C1C615A6BF2A}" uniqueName="5" name="SKU_DESCRIPTION" queryTableFieldId="21" dataDxfId="8"/>
+    <tableColumn id="9" xr3:uid="{AE09184F-0511-4178-958B-3187FE75758F}" uniqueName="9" name="DATE_SUBMISSION" queryTableFieldId="20" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{CF6A5C58-AABF-4AE9-B345-C4F3D9736768}" name="Table1" displayName="Table1" ref="C6:F7" totalsRowShown="0">
+  <autoFilter ref="C6:F7" xr:uid="{0913F4EF-D9E4-40C6-96BF-F818F82EBF09}"/>
+  <tableColumns count="4">
+    <tableColumn id="1" xr3:uid="{FEDA7D8A-C95C-44BC-ADBF-2EC2A09C62E9}" name="max oh date" dataDxfId="6">
+      <calculatedColumnFormula>MAX(OUTPUT[OH_DATE])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{1D4835E2-146E-445E-8B70-984C3B5C7EF7}" name="today" dataDxfId="5">
+      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{F6A0C73A-990E-44F9-9361-20AB2711F921}" name="diff">
+      <calculatedColumnFormula>D7-C7</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{A0785B66-2E2C-4366-A5C0-5E3301EAD807}" name="is within 7 days">
+      <calculatedColumnFormula>AND(E7&gt;= 0, E7&lt;=7)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{F5F98B10-3E49-4FCB-9961-285798799925}" name="Table3" displayName="Table3" ref="C10:E11" totalsRowShown="0">
+  <autoFilter ref="C10:E11" xr:uid="{992D282B-DE81-4ED3-9E4B-1F3AECFD0A8C}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{112CF9F0-B0BE-412B-8618-125B232E3BC3}" name="record count">
+      <calculatedColumnFormula>COUNTA(OUTPUT[SKU])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{F575566E-7FB6-4255-9BE1-CCAA985E8019}" name="counta(oh date)">
+      <calculatedColumnFormula>COUNTA(OUTPUT[OH_DATE])</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{43FBD581-55E8-4129-840C-C9F98322DC53}" name="Column1">
+      <calculatedColumnFormula>D11=C11</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -4774,9 +5133,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6186D433-10DE-487E-82BC-BD5E185B1B11}">
   <dimension ref="A1:H1326"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G6" sqref="G6"/>
+      <selection pane="bottomLeft" activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -37185,6 +37544,124 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{23B16794-BD5E-4A7B-827A-12775CB8F684}">
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="3" max="3" width="13" customWidth="1"/>
+    <col min="4" max="4" width="15.6640625" customWidth="1"/>
+    <col min="5" max="5" width="9.86328125" customWidth="1"/>
+    <col min="6" max="6" width="15.19921875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="A1" s="3" t="b">
+        <f ca="1">AND(E11,F7)</f>
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1421</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D2" t="s">
+        <v>1422</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E3" t="s">
+        <v>1423</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="D4" t="s">
+        <v>1424</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C6" t="s">
+        <v>1425</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1426</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1427</v>
+      </c>
+      <c r="F6" t="s">
+        <v>1428</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C7" s="4">
+        <f>MAX(OUTPUT[OH_DATE])</f>
+        <v>44241</v>
+      </c>
+      <c r="D7" s="2">
+        <f ca="1">TODAY()</f>
+        <v>44248</v>
+      </c>
+      <c r="E7">
+        <f ca="1">D7-C7</f>
+        <v>7</v>
+      </c>
+      <c r="F7" t="b">
+        <f ca="1">AND(E7&gt;= 0, E7&lt;=7)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C10" t="s">
+        <v>1429</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1430</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1431</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="C11">
+        <f>COUNTA(OUTPUT[SKU])</f>
+        <v>1325</v>
+      </c>
+      <c r="D11">
+        <f>COUNTA(OUTPUT[OH_DATE])</f>
+        <v>909</v>
+      </c>
+      <c r="E11" t="b">
+        <f>D11=C11</f>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="F7 E11">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+      <formula>TRUE</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>FALSE</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="2">
+    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B48CAD5-A998-444F-A470-1C46138E9EEE}">
   <dimension ref="A1"/>
   <sheetViews>

</xml_diff>